<commit_message>
Modify MFG and PCB design files
</commit_message>
<xml_diff>
--- a/BOM/sophum_esc_v3.xlsx
+++ b/BOM/sophum_esc_v3.xlsx
@@ -51,9 +51,6 @@
     <t>22uF</t>
   </si>
   <si>
-    <t>C0805</t>
-  </si>
-  <si>
     <t>C7,C8,C9</t>
   </si>
   <si>
@@ -170,10 +167,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>嘉立创元件表号</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>C72339</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -221,6 +214,14 @@
   </si>
   <si>
     <t>NONE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>嘉立创元件编号</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC0805</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -228,7 +229,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,6 +400,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="134"/>
@@ -829,7 +838,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -837,6 +846,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -887,19 +899,6 @@
   <dxfs count="7">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -918,11 +917,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -932,11 +927,10 @@
         <name val="微软雅黑"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1006,6 +1000,24 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1020,14 +1032,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E18" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E18" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E18"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Comment" dataDxfId="6"/>
-    <tableColumn id="2" name="Designator" dataDxfId="5"/>
+    <tableColumn id="1" name="Comment" dataDxfId="4"/>
+    <tableColumn id="2" name="Designator" dataDxfId="3"/>
     <tableColumn id="3" name="Footprint" dataDxfId="2"/>
-    <tableColumn id="4" name="嘉立创元件表号" dataDxfId="0"/>
-    <tableColumn id="5" name="Quantity" dataDxfId="1"/>
+    <tableColumn id="4" name="嘉立创元件编号" dataDxfId="1"/>
+    <tableColumn id="5" name="Quantity" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1299,7 +1311,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1313,16 +1325,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -1339,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1">
         <v>4</v>
@@ -1356,7 +1368,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1370,10 +1382,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1381,16 +1393,16 @@
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
@@ -1398,16 +1410,16 @@
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>65</v>
+      <c r="D6" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -1415,16 +1427,16 @@
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>65</v>
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -1432,16 +1444,16 @@
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -1449,16 +1461,16 @@
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -1466,16 +1478,16 @@
     </row>
     <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E10" s="1">
         <v>3</v>
@@ -1483,16 +1495,16 @@
     </row>
     <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1">
         <v>3</v>
@@ -1500,16 +1512,16 @@
     </row>
     <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
@@ -1517,16 +1529,16 @@
     </row>
     <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" s="1">
         <v>8</v>
@@ -1534,16 +1546,16 @@
     </row>
     <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1">
         <v>4</v>
@@ -1551,16 +1563,16 @@
     </row>
     <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E15" s="1">
         <v>3</v>
@@ -1568,16 +1580,16 @@
     </row>
     <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1">
         <v>6</v>
@@ -1585,16 +1597,16 @@
     </row>
     <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -1602,16 +1614,16 @@
     </row>
     <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>

</xml_diff>